<commit_message>
-Update the pcb layout design to be based on 4 layers for better performance and improve the analog design
</commit_message>
<xml_diff>
--- a/H2AR32/Release/BOM/H2AR32.xlsx
+++ b/H2AR32/Release/BOM/H2AR32.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H2AR3x-Hardware\H2AR32\Release\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698F926C-BDF5-4454-9DFB-9A92ECE41D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFAC894-265C-4AF2-A4AF-BF5BD77C1A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="143">
   <si>
     <t>Description</t>
   </si>
@@ -91,18 +91,9 @@
     <t>Vishay</t>
   </si>
   <si>
-    <t>PCB Header, Unshrouded, Thru 02 Straight Header, .101, AMPMODU Mod II Series</t>
-  </si>
-  <si>
     <t>TE Connectivity</t>
   </si>
   <si>
-    <t>87227-1</t>
-  </si>
-  <si>
-    <t>https://octopart.com/87227-1-te+connectivity-39512052?r=sp</t>
-  </si>
-  <si>
     <t>Conn Unshrouded Header HDR 3 POS 2.54mm Solder ST Top Entry Thru-Hole Carton</t>
   </si>
   <si>
@@ -112,18 +103,12 @@
     <t>https://octopart.com/5-146281-3-te+connectivity+%2F+amp-39745942?r=sp</t>
   </si>
   <si>
-    <t>YAGEO [VA]</t>
-  </si>
-  <si>
     <t>CC0805KKX7R7BB105</t>
   </si>
   <si>
     <t>https://octopart.com/cc0805kkx7r7bb105-yageo-8376555?r=sp</t>
   </si>
   <si>
-    <t>YAGEO [VR]</t>
-  </si>
-  <si>
     <t>ERJ-3GEYJ271V</t>
   </si>
   <si>
@@ -334,18 +319,9 @@
     <t>C11, C12, C17, C18</t>
   </si>
   <si>
-    <t>REF2033AIDDCR</t>
-  </si>
-  <si>
-    <t>https://octopart.com/ref2033aiddcr-texas+instruments-46921199?r=sp</t>
-  </si>
-  <si>
     <t>U4</t>
   </si>
   <si>
-    <t>Low-Drift, Low-Power, Dual-Output Vref and Vref/2 Voltage Reference 5-SOT-23-THIN -40 to 125</t>
-  </si>
-  <si>
     <t>C10 , C16</t>
   </si>
   <si>
@@ -391,27 +367,6 @@
     <t>C1,C2,C9</t>
   </si>
   <si>
-    <t>C3, C5, C6, C8, C13, C14, C15, C19, C21, C22, C23</t>
-  </si>
-  <si>
-    <t>CRCW0603150RFKEA</t>
-  </si>
-  <si>
-    <t>https://octopart.com/crcw0603150rfkea-vishay-39455211</t>
-  </si>
-  <si>
-    <t>RES SMD 150 OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>RC0603JR-071ML</t>
-  </si>
-  <si>
-    <t>https://octopart.com/rc0603jr-071ml-yageo-40254917?r=sp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Res Thick Film 0603 1M Ohm 5% 1/10W ±100ppm/°C </t>
-  </si>
-  <si>
     <t>Y14870R10000B9R</t>
   </si>
   <si>
@@ -458,13 +413,55 @@
   </si>
   <si>
     <t>https://octopart.com/cr8401-1000-g-cr+magnetics-1366028?r=sp</t>
+  </si>
+  <si>
+    <t>Headers &amp; Wire Housings Unshrouded 1 POS T/H</t>
+  </si>
+  <si>
+    <t>5-146280-1</t>
+  </si>
+  <si>
+    <t>https://octopart.com/5-146280-1-te+connectivity+%2F+amp-40259676?r=sp</t>
+  </si>
+  <si>
+    <t>C3, C5, C6, C8, C13, C14, C15, C19, C20 , C21, C22, C23</t>
+  </si>
+  <si>
+    <t>RES SMD 150 OHM 0,1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t>ERA-8AEB151V</t>
+  </si>
+  <si>
+    <t>https://octopart.com/era-8aeb151v-panasonic-55477439?r=sp</t>
+  </si>
+  <si>
+    <t>RES SMD 1M OHM 0,1% 1/4W 1206</t>
+  </si>
+  <si>
+    <t>RT1206BRD071ML</t>
+  </si>
+  <si>
+    <t>YAGEO</t>
+  </si>
+  <si>
+    <t>https://octopart.com/rt1206brd071ml-yageo-1262221?r=sp</t>
+  </si>
+  <si>
+    <t>REF2030AIDDCT</t>
+  </si>
+  <si>
+    <t>https://octopart.com/ref2030aiddct-texas+instruments-46921198?r=sp</t>
+  </si>
+  <si>
+    <t>3-V Vref, low-drift, low-power, dual-output Vref &amp; Vref/2 voltage reference 5-SOT-23</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -507,12 +504,6 @@
     </font>
     <font>
       <b/>
-      <sz val="28"/>
-      <name val="Trebuchet MS"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -682,9 +673,8 @@
       <u/>
       <sz val="9"/>
       <color theme="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -874,7 +864,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1054,53 +1044,66 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1108,57 +1111,41 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1181,6 +1168,39 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1252,15 +1272,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
+      <xdr:colOff>393700</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>173788</xdr:rowOff>
+      <xdr:rowOff>149975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2174599</xdr:colOff>
+      <xdr:colOff>2146478</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:rowOff>-1</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1288,8 +1308,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="171450" y="173788"/>
-          <a:ext cx="2905125" cy="616787"/>
+          <a:off x="393700" y="149975"/>
+          <a:ext cx="2975153" cy="604087"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1598,20 +1618,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G37"/>
+  <dimension ref="A2:GV37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.69921875" customWidth="1"/>
-    <col min="2" max="2" width="70.59765625" customWidth="1"/>
-    <col min="3" max="3" width="21.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="84" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.3984375" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="56.69921875" customWidth="1"/>
+    <col min="3" max="3" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.09765625" customWidth="1"/>
+    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="49" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1622,8 +1642,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="8"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="14" t="s">
+      <c r="E2" s="31" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1633,8 +1652,8 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="12"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
     </row>
     <row r="4" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
@@ -1646,11 +1665,11 @@
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="16">
         <v>2</v>
       </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -1658,16 +1677,16 @@
         <v>9</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="17">
         <v>45195</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="25"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="19"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -1675,14 +1694,14 @@
         <v>10</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="28"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="22"/>
       <c r="G6" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -1692,10 +1711,10 @@
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -1706,563 +1725,839 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="F9" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="F11" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="F13" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="F15" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="F17" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="F19" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="E20" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="F20" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="E23" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="F27" s="14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="16">
+      <c r="B29" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="F29" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="16">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="F31" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="F11" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="F12" s="16">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E32" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="F32" s="14">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="C13" s="15" t="s">
+    <row r="33" spans="1:204" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A33" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E33" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="F33" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:204" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" s="15">
+        <v>1</v>
+      </c>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="27"/>
+      <c r="L34" s="27"/>
+      <c r="M34" s="27"/>
+      <c r="N34" s="27"/>
+      <c r="O34" s="27"/>
+      <c r="P34" s="27"/>
+      <c r="Q34" s="27"/>
+      <c r="R34" s="27"/>
+      <c r="S34" s="27"/>
+      <c r="T34" s="27"/>
+      <c r="U34" s="27"/>
+      <c r="V34" s="27"/>
+      <c r="W34" s="27"/>
+      <c r="X34" s="27"/>
+      <c r="Y34" s="27"/>
+      <c r="Z34" s="27"/>
+      <c r="AA34" s="27"/>
+      <c r="AB34" s="27"/>
+      <c r="AC34" s="27"/>
+      <c r="AD34" s="27"/>
+      <c r="AE34" s="27"/>
+      <c r="AF34" s="27"/>
+      <c r="AG34" s="27"/>
+      <c r="AH34" s="27"/>
+      <c r="AI34" s="27"/>
+      <c r="AJ34" s="27"/>
+      <c r="AK34" s="27"/>
+      <c r="AL34" s="27"/>
+      <c r="AM34" s="27"/>
+      <c r="AN34" s="27"/>
+      <c r="AO34" s="27"/>
+      <c r="AP34" s="27"/>
+      <c r="AQ34" s="27"/>
+      <c r="AR34" s="27"/>
+      <c r="AS34" s="27"/>
+      <c r="AT34" s="27"/>
+      <c r="AU34" s="27"/>
+      <c r="AV34" s="27"/>
+      <c r="AW34" s="27"/>
+      <c r="AX34" s="27"/>
+      <c r="AY34" s="27"/>
+      <c r="AZ34" s="27"/>
+      <c r="BA34" s="27"/>
+      <c r="BB34" s="27"/>
+      <c r="BC34" s="27"/>
+      <c r="BD34" s="27"/>
+      <c r="BE34" s="27"/>
+      <c r="BF34" s="27"/>
+      <c r="BG34" s="27"/>
+      <c r="BH34" s="27"/>
+      <c r="BI34" s="27"/>
+      <c r="BJ34" s="27"/>
+      <c r="BK34" s="27"/>
+      <c r="BL34" s="27"/>
+      <c r="BM34" s="27"/>
+      <c r="BN34" s="27"/>
+      <c r="BO34" s="27"/>
+      <c r="BP34" s="27"/>
+      <c r="BQ34" s="27"/>
+      <c r="BR34" s="27"/>
+      <c r="BS34" s="27"/>
+      <c r="BT34" s="27"/>
+      <c r="BU34" s="27"/>
+      <c r="BV34" s="27"/>
+      <c r="BW34" s="27"/>
+      <c r="BX34" s="27"/>
+      <c r="BY34" s="27"/>
+      <c r="BZ34" s="27"/>
+      <c r="CA34" s="27"/>
+      <c r="CB34" s="27"/>
+      <c r="CC34" s="27"/>
+      <c r="CD34" s="27"/>
+      <c r="CE34" s="27"/>
+      <c r="CF34" s="27"/>
+      <c r="CG34" s="27"/>
+      <c r="CH34" s="27"/>
+      <c r="CI34" s="27"/>
+      <c r="CJ34" s="27"/>
+      <c r="CK34" s="27"/>
+      <c r="CL34" s="27"/>
+      <c r="CM34" s="27"/>
+      <c r="CN34" s="27"/>
+      <c r="CO34" s="27"/>
+      <c r="CP34" s="27"/>
+      <c r="CQ34" s="27"/>
+      <c r="CR34" s="27"/>
+      <c r="CS34" s="27"/>
+      <c r="CT34" s="27"/>
+      <c r="CU34" s="27"/>
+      <c r="CV34" s="27"/>
+      <c r="CW34" s="27"/>
+      <c r="CX34" s="27"/>
+      <c r="CY34" s="27"/>
+      <c r="CZ34" s="27"/>
+      <c r="DA34" s="27"/>
+      <c r="DB34" s="27"/>
+      <c r="DC34" s="27"/>
+      <c r="DD34" s="27"/>
+      <c r="DE34" s="27"/>
+      <c r="DF34" s="27"/>
+      <c r="DG34" s="27"/>
+      <c r="DH34" s="27"/>
+      <c r="DI34" s="27"/>
+      <c r="DJ34" s="27"/>
+      <c r="DK34" s="27"/>
+      <c r="DL34" s="27"/>
+      <c r="DM34" s="27"/>
+      <c r="DN34" s="27"/>
+      <c r="DO34" s="27"/>
+      <c r="DP34" s="27"/>
+      <c r="DQ34" s="27"/>
+      <c r="DR34" s="27"/>
+      <c r="DS34" s="27"/>
+      <c r="DT34" s="27"/>
+      <c r="DU34" s="27"/>
+      <c r="DV34" s="27"/>
+      <c r="DW34" s="27"/>
+      <c r="DX34" s="27"/>
+      <c r="DY34" s="27"/>
+      <c r="DZ34" s="27"/>
+      <c r="EA34" s="27"/>
+      <c r="EB34" s="27"/>
+      <c r="EC34" s="27"/>
+      <c r="ED34" s="27"/>
+      <c r="EE34" s="27"/>
+      <c r="EF34" s="27"/>
+      <c r="EG34" s="27"/>
+      <c r="EH34" s="27"/>
+      <c r="EI34" s="27"/>
+      <c r="EJ34" s="27"/>
+      <c r="EK34" s="27"/>
+      <c r="EL34" s="27"/>
+      <c r="EM34" s="27"/>
+      <c r="EN34" s="27"/>
+      <c r="EO34" s="27"/>
+      <c r="EP34" s="27"/>
+      <c r="EQ34" s="27"/>
+      <c r="ER34" s="27"/>
+      <c r="ES34" s="27"/>
+      <c r="ET34" s="27"/>
+      <c r="EU34" s="27"/>
+      <c r="EV34" s="27"/>
+      <c r="EW34" s="27"/>
+      <c r="EX34" s="27"/>
+      <c r="EY34" s="27"/>
+      <c r="EZ34" s="27"/>
+      <c r="FA34" s="27"/>
+      <c r="FB34" s="27"/>
+      <c r="FC34" s="27"/>
+      <c r="FD34" s="27"/>
+      <c r="FE34" s="27"/>
+      <c r="FF34" s="27"/>
+      <c r="FG34" s="27"/>
+      <c r="FH34" s="27"/>
+      <c r="FI34" s="27"/>
+      <c r="FJ34" s="27"/>
+      <c r="FK34" s="27"/>
+      <c r="FL34" s="27"/>
+      <c r="FM34" s="27"/>
+      <c r="FN34" s="27"/>
+      <c r="FO34" s="27"/>
+      <c r="FP34" s="27"/>
+      <c r="FQ34" s="27"/>
+      <c r="FR34" s="27"/>
+      <c r="FS34" s="27"/>
+      <c r="FT34" s="27"/>
+      <c r="FU34" s="27"/>
+      <c r="FV34" s="27"/>
+      <c r="FW34" s="27"/>
+      <c r="FX34" s="27"/>
+      <c r="FY34" s="27"/>
+      <c r="FZ34" s="27"/>
+      <c r="GA34" s="27"/>
+      <c r="GB34" s="27"/>
+      <c r="GC34" s="27"/>
+      <c r="GD34" s="27"/>
+      <c r="GE34" s="27"/>
+      <c r="GF34" s="27"/>
+      <c r="GG34" s="27"/>
+      <c r="GH34" s="27"/>
+      <c r="GI34" s="27"/>
+      <c r="GJ34" s="27"/>
+      <c r="GK34" s="27"/>
+      <c r="GL34" s="27"/>
+      <c r="GM34" s="27"/>
+      <c r="GN34" s="27"/>
+      <c r="GO34" s="27"/>
+      <c r="GP34" s="27"/>
+      <c r="GQ34" s="27"/>
+      <c r="GR34" s="27"/>
+      <c r="GS34" s="27"/>
+      <c r="GT34" s="27"/>
+      <c r="GU34" s="27"/>
+      <c r="GV34" s="27"/>
+    </row>
+    <row r="35" spans="1:204" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="26"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="34"/>
+    </row>
+    <row r="36" spans="1:204" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E36" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="F36" s="14">
+        <v>1</v>
+      </c>
+      <c r="G36" s="27"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="27"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="27"/>
+      <c r="L36" s="27"/>
+      <c r="M36" s="27"/>
+      <c r="N36" s="27"/>
+      <c r="O36" s="27"/>
+      <c r="P36" s="27"/>
+      <c r="Q36" s="27"/>
+      <c r="R36" s="27"/>
+      <c r="S36" s="27"/>
+      <c r="T36" s="27"/>
+      <c r="U36" s="27"/>
+      <c r="V36" s="27"/>
+      <c r="W36" s="27"/>
+      <c r="X36" s="27"/>
+      <c r="Y36" s="27"/>
+      <c r="Z36" s="27"/>
+      <c r="AA36" s="27"/>
+      <c r="AB36" s="27"/>
+      <c r="AC36" s="27"/>
+      <c r="AD36" s="27"/>
+      <c r="AE36" s="27"/>
+      <c r="AF36" s="27"/>
+      <c r="AG36" s="27"/>
+      <c r="AH36" s="27"/>
+      <c r="AI36" s="27"/>
+      <c r="AJ36" s="27"/>
+      <c r="AK36" s="27"/>
+      <c r="AL36" s="27"/>
+      <c r="AM36" s="27"/>
+      <c r="AN36" s="27"/>
+      <c r="AO36" s="27"/>
+      <c r="AP36" s="27"/>
+      <c r="AQ36" s="27"/>
+      <c r="AR36" s="27"/>
+      <c r="AS36" s="27"/>
+      <c r="AT36" s="27"/>
+      <c r="AU36" s="27"/>
+      <c r="AV36" s="27"/>
+      <c r="AW36" s="27"/>
+      <c r="AX36" s="27"/>
+      <c r="AY36" s="27"/>
+      <c r="AZ36" s="27"/>
+      <c r="BA36" s="27"/>
+      <c r="BB36" s="27"/>
+      <c r="BC36" s="27"/>
+      <c r="BD36" s="27"/>
+      <c r="BE36" s="27"/>
+      <c r="BF36" s="27"/>
+      <c r="BG36" s="27"/>
+      <c r="BH36" s="27"/>
+      <c r="BI36" s="27"/>
+      <c r="BJ36" s="27"/>
+      <c r="BK36" s="27"/>
+      <c r="BL36" s="27"/>
+      <c r="BM36" s="27"/>
+      <c r="BN36" s="27"/>
+      <c r="BO36" s="27"/>
+      <c r="BP36" s="27"/>
+      <c r="BQ36" s="27"/>
+      <c r="BR36" s="27"/>
+      <c r="BS36" s="27"/>
+      <c r="BT36" s="27"/>
+      <c r="BU36" s="27"/>
+      <c r="BV36" s="27"/>
+      <c r="BW36" s="27"/>
+      <c r="BX36" s="27"/>
+      <c r="BY36" s="30"/>
+    </row>
+    <row r="37" spans="1:204" x14ac:dyDescent="0.25">
+      <c r="A37" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="B37" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="C37" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="D37" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="E37" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="D13" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="F13" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="F14" s="16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="F15" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="F17" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="F18" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="F19" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="F20" s="16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
+      <c r="F37" s="25" t="s">
         <v>121</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="F21" s="16">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="F22" s="16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="F23" s="16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" s="16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="F25" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="E26" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F26" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="E27" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="F27" s="16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E28" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F28" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="E29" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="F29" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E30" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="F30" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="E31" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="F31" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="E32" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="F32" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="E33" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="F33" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E34" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="F34" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="E36" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="F36" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="D37" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="E37" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="F37" s="16" t="s">
-        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2272,20 +2567,20 @@
     <mergeCell ref="D6:F6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E24" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E26" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E30" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E28" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E34" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E16" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="E10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E18" r:id="rId9" xr:uid="{BC208596-CFFC-4841-9008-85FEAC1F1913}"/>
-    <hyperlink ref="E21" r:id="rId10" xr:uid="{608D9BE0-DE64-484B-BD24-E5CEAA1C46E2}"/>
-    <hyperlink ref="E25" r:id="rId11" xr:uid="{8247B2C4-59B6-4E38-8F18-15A37292F9D6}"/>
-    <hyperlink ref="E12" r:id="rId12" xr:uid="{3F162551-9AAC-4522-AC2E-98D734B996E5}"/>
-    <hyperlink ref="E22" r:id="rId13" xr:uid="{B203383E-1301-4B5F-B98D-4D004B0B5327}"/>
-    <hyperlink ref="E23" r:id="rId14" xr:uid="{84C39794-A596-4142-9E81-ABDD3DE38303}"/>
+    <hyperlink ref="E24" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E26" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E30" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E28" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E34" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E16" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E18" r:id="rId8" xr:uid="{BC208596-CFFC-4841-9008-85FEAC1F1913}"/>
+    <hyperlink ref="E21" r:id="rId9" xr:uid="{608D9BE0-DE64-484B-BD24-E5CEAA1C46E2}"/>
+    <hyperlink ref="E25" r:id="rId10" xr:uid="{8247B2C4-59B6-4E38-8F18-15A37292F9D6}"/>
+    <hyperlink ref="E12" r:id="rId11" xr:uid="{3F162551-9AAC-4522-AC2E-98D734B996E5}"/>
+    <hyperlink ref="E22" r:id="rId12" xr:uid="{B203383E-1301-4B5F-B98D-4D004B0B5327}"/>
+    <hyperlink ref="E23" r:id="rId13" xr:uid="{84C39794-A596-4142-9E81-ABDD3DE38303}"/>
+    <hyperlink ref="E20" r:id="rId14" xr:uid="{56AE25A4-CDDA-4DEB-B9D8-D659BF0D2AA3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId15"/>

</xml_diff>